<commit_message>
Auto and Shuttling Changes
</commit_message>
<xml_diff>
--- a/FRC5010_2024/Calibration/Auto Aim Calibration.xlsx
+++ b/FRC5010_2024/Calibration/Auto Aim Calibration.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\FRCLibrary\FRC5010_2024\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7563E1F4-2399-4F68-AFB7-60EBB6CA7A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{54B7F906-B4D3-4E56-ABF1-EE9F7A23D4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5325" yWindow="-16200" windowWidth="19410" windowHeight="15585" xr2:uid="{B93A0FFF-B288-4807-B24E-5C9046F798FA}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" xr2:uid="{B93A0FFF-B288-4807-B24E-5C9046F798FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>X</t>
   </si>
@@ -48,9 +49,6 @@
   </si>
   <si>
     <t>Shooter Speed</t>
-  </si>
-  <si>
-    <t>Column1</t>
   </si>
   <si>
     <t>Distance to Speaker</t>
@@ -125,23 +123,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A36C3B9E-0966-4F13-B2E3-F6116C5EBF0D}" name="Table1" displayName="Table1" ref="A1:G1048576" totalsRowShown="0">
-  <autoFilter ref="A1:G1048576" xr:uid="{A36C3B9E-0966-4F13-B2E3-F6116C5EBF0D}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{42C266CC-5422-4C5B-935F-DB4096B74230}" name="X"/>
-    <tableColumn id="7" xr3:uid="{E5955C81-D37C-4788-BA57-40BDF0F113AD}" name="Y"/>
-    <tableColumn id="8" xr3:uid="{D271585F-5787-4438-9FBA-75C4A5DAB8C1}" name="Distance to Speaker"/>
-    <tableColumn id="2" xr3:uid="{BA8D2532-12EC-4C58-9614-FE6677AA5355}" name="Pivot Angle"/>
-    <tableColumn id="3" xr3:uid="{350061EE-BC36-4750-A449-5D25B820AD19}" name="Pivot Reference"/>
-    <tableColumn id="4" xr3:uid="{8917E9D4-D0B4-46C1-AA35-6A8FADA43042}" name="Shooter Speed"/>
-    <tableColumn id="9" xr3:uid="{70D1F80F-E126-40FF-AE31-7F3A4B8ED7E3}" name="From Where Description"/>
-    <tableColumn id="5" xr3:uid="{2647E056-0BDC-4FCB-B076-6D784EE4057B}" name="Date - 4/10/2024"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -466,22 +447,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -501,7 +482,7 @@
         <v>-9.8000000000000007</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -824,7 +805,7 @@
         <v>3520.4296875</v>
       </c>
       <c r="G18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -867,14 +848,11 @@
         <v>3492.1875</v>
       </c>
       <c r="G20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>